<commit_message>
binary experiments wit DL and Scikit
</commit_message>
<xml_diff>
--- a/data/buzzfeed-debunk-combined/visualization.xlsx
+++ b/data/buzzfeed-debunk-combined/visualization.xlsx
@@ -15,6 +15,7 @@
     <sheet name="CNN1 1000" sheetId="6" r:id="rId6"/>
     <sheet name="CNN2 1000" sheetId="7" r:id="rId7"/>
     <sheet name="CNN binary" sheetId="8" r:id="rId8"/>
+    <sheet name="TF-IDF" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19965,4 +19966,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
visualization file almost complete
</commit_message>
<xml_diff>
--- a/data/buzzfeed-debunk-combined/visualization.xlsx
+++ b/data/buzzfeed-debunk-combined/visualization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="rashkin classifier" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="CNN1 1000" sheetId="6" r:id="rId6"/>
     <sheet name="CNN2 1000" sheetId="7" r:id="rId7"/>
     <sheet name="CNN binary" sheetId="8" r:id="rId8"/>
-    <sheet name="TF-IDF" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet7" sheetId="10" r:id="rId10"/>
+    <sheet name="binary extra" sheetId="11" r:id="rId9"/>
+    <sheet name="TF-IDF" sheetId="9" r:id="rId10"/>
+    <sheet name="Sheet7" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="393">
   <si>
     <t xml:space="preserve">ftrue </t>
   </si>
@@ -4179,6 +4180,102 @@
   </si>
   <si>
     <t>TF-IDF SVC</t>
+  </si>
+  <si>
+    <t>CNN 1 model:</t>
+  </si>
+  <si>
+    <t>CNN 2 model:</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 16 : [0.10360931873321533, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.7204475677013398, 0.77]</t>
+  </si>
+  <si>
+    <t>[0.803442873954773, 0.7375]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 19 : [0.16020009228161403, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.7711168563365937, 0.77]</t>
+  </si>
+  <si>
+    <t>[0.8235645294189453, 0.74375]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 15 : [0.13102907759802682, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.7690710926055908, 0.76]</t>
+  </si>
+  <si>
+    <t>[0.799694230556488, 0.735]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 14 : [0.1286380693742207, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.739014436006546, 0.75625]</t>
+  </si>
+  <si>
+    <t>[0.7659110426902771, 0.74625]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 13 : [0.16592042693070003, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.7652655279636383, 0.76375]</t>
+  </si>
+  <si>
+    <t>[0.7834830844402313, 0.7475]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 16 : [0.022870092482439108, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.8932331466674804, 0.7375]</t>
+  </si>
+  <si>
+    <t>[0.9303717708587647, 0.71625]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 10 : [0.06033183059522084, 0.9942857142857143]</t>
+  </si>
+  <si>
+    <t>[0.7692045044898986, 0.73]</t>
+  </si>
+  <si>
+    <t>[0.7739324069023132, 0.71875]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 12 : [0.026289071972881044, 0.9967857142857143]</t>
+  </si>
+  <si>
+    <t>[1.1035455417633058, 0.73625]</t>
+  </si>
+  <si>
+    <t>[1.150442715883255, 0.715]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 15 : [0.02318094883646284, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[0.921134819984436, 0.73125]</t>
+  </si>
+  <si>
+    <t>[0.945082014799118, 0.73125]</t>
+  </si>
+  <si>
+    <t>Best accuracy found at epoch 17 : [0.02062257977468627, 0.9982142857142857]</t>
+  </si>
+  <si>
+    <t>[1.0735913491249085, 0.74625]</t>
+  </si>
+  <si>
+    <t>[1.1316575944423675, 0.7175]</t>
   </si>
 </sst>
 </file>
@@ -14660,9 +14757,95 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" t="s">
+        <v>331</v>
+      </c>
+      <c r="G3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H3" t="s">
+        <v>328</v>
+      </c>
+      <c r="I3" t="s">
+        <v>333</v>
+      </c>
+      <c r="J3" t="s">
+        <v>334</v>
+      </c>
+      <c r="K3" t="s">
+        <v>333</v>
+      </c>
+      <c r="L3" t="s">
+        <v>335</v>
+      </c>
+      <c r="M3" t="s">
+        <v>336</v>
+      </c>
+      <c r="N3" t="s">
+        <v>328</v>
+      </c>
+      <c r="O3" t="s">
+        <v>337</v>
+      </c>
+      <c r="P3" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>337</v>
+      </c>
+      <c r="R3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -19729,15 +19912,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32:M33"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="18" max="18" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -20177,303 +20361,20 @@
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>296</v>
-      </c>
-    </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>273</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
+        <v>273</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20">
-        <v>16</v>
-      </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" t="s">
-        <v>297</v>
-      </c>
-      <c r="I20">
-        <v>0.99821428571428505</v>
-      </c>
-      <c r="J20" t="s">
-        <v>298</v>
-      </c>
-      <c r="K20">
-        <v>0.76749999999999996</v>
-      </c>
-      <c r="L20" t="s">
-        <v>299</v>
-      </c>
-      <c r="M20">
-        <v>0.74250000000000005</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" t="s">
-        <v>300</v>
-      </c>
-      <c r="I21">
-        <v>0.99821428571428505</v>
-      </c>
-      <c r="J21" t="s">
-        <v>301</v>
-      </c>
-      <c r="K21">
-        <v>0.77249999999999996</v>
-      </c>
-      <c r="L21" t="s">
-        <v>302</v>
-      </c>
-      <c r="M21">
-        <v>0.72875000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22">
-        <v>16</v>
-      </c>
-      <c r="G22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" t="s">
-        <v>303</v>
-      </c>
-      <c r="I22">
-        <v>0.99821428571428505</v>
-      </c>
-      <c r="J22" t="s">
-        <v>304</v>
-      </c>
-      <c r="K22">
-        <v>0.76124999999999998</v>
-      </c>
-      <c r="L22" t="s">
-        <v>305</v>
-      </c>
-      <c r="M22">
-        <v>0.73875000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23">
-        <v>17</v>
-      </c>
-      <c r="G23" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" t="s">
-        <v>306</v>
-      </c>
-      <c r="I23">
-        <v>0.997857142857142</v>
-      </c>
-      <c r="J23" t="s">
-        <v>307</v>
-      </c>
-      <c r="K23">
-        <v>0.75749999999999995</v>
-      </c>
-      <c r="L23" t="s">
-        <v>308</v>
-      </c>
-      <c r="M23">
-        <v>0.75124999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24">
-        <v>16</v>
-      </c>
-      <c r="G24" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" t="s">
-        <v>309</v>
-      </c>
-      <c r="I24">
-        <v>0.99821428571428505</v>
-      </c>
-      <c r="J24" t="s">
-        <v>310</v>
-      </c>
-      <c r="K24">
-        <v>0.77124999999999999</v>
-      </c>
-      <c r="L24" t="s">
-        <v>311</v>
-      </c>
-      <c r="M24">
-        <v>0.74124999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K25">
-        <f>AVERAGE(K20:K24)</f>
-        <v>0.76600000000000001</v>
-      </c>
-      <c r="L25" t="e">
-        <f t="shared" ref="L25:M25" si="0">AVERAGE(L20:L24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="0"/>
-        <v>0.74049999999999994</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>273</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
         <v>274</v>
-      </c>
-      <c r="K26">
-        <f>STDEV(K20:K24)</f>
-        <v>6.4590053413819126E-3</v>
-      </c>
-      <c r="L26" t="e">
-        <f t="shared" ref="L26:M26" si="1">STDEV(L20:L24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="1"/>
-        <v>8.0816149376222949E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27">
-        <v>14</v>
-      </c>
-      <c r="G27" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" t="s">
-        <v>312</v>
-      </c>
-      <c r="I27">
-        <v>0.99821428571428505</v>
-      </c>
-      <c r="J27" t="s">
-        <v>313</v>
-      </c>
-      <c r="K27">
-        <v>0.72375</v>
-      </c>
-      <c r="L27" t="s">
-        <v>314</v>
-      </c>
-      <c r="M27">
-        <v>0.71499999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -20493,28 +20394,28 @@
         <v>39</v>
       </c>
       <c r="F28">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G28" t="s">
         <v>40</v>
       </c>
       <c r="H28" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="I28">
-        <v>0.996428571428571</v>
+        <v>0.99821428571428505</v>
       </c>
       <c r="J28" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="K28">
-        <v>0.72875000000000001</v>
+        <v>0.76749999999999996</v>
       </c>
       <c r="L28" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="M28">
-        <v>0.73375000000000001</v>
+        <v>0.74250000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -20534,28 +20435,28 @@
         <v>39</v>
       </c>
       <c r="F29">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G29" t="s">
         <v>40</v>
       </c>
       <c r="H29" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="I29">
-        <v>0.997857142857142</v>
+        <v>0.99821428571428505</v>
       </c>
       <c r="J29" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="K29">
-        <v>0.73375000000000001</v>
+        <v>0.77249999999999996</v>
       </c>
       <c r="L29" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="M29">
-        <v>0.70625000000000004</v>
+        <v>0.72875000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -20575,28 +20476,28 @@
         <v>39</v>
       </c>
       <c r="F30">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
         <v>40</v>
       </c>
       <c r="H30" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="I30">
-        <v>0.997857142857142</v>
+        <v>0.99821428571428505</v>
       </c>
       <c r="J30" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="K30">
-        <v>0.74375000000000002</v>
+        <v>0.76124999999999998</v>
       </c>
       <c r="L30" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="M30">
-        <v>0.73250000000000004</v>
+        <v>0.73875000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -20616,54 +20517,339 @@
         <v>39</v>
       </c>
       <c r="F31">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
         <v>40</v>
       </c>
       <c r="H31" t="s">
+        <v>306</v>
+      </c>
+      <c r="I31">
+        <v>0.997857142857142</v>
+      </c>
+      <c r="J31" t="s">
+        <v>307</v>
+      </c>
+      <c r="K31">
+        <v>0.75749999999999995</v>
+      </c>
+      <c r="L31" t="s">
+        <v>308</v>
+      </c>
+      <c r="M31">
+        <v>0.75124999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s">
+        <v>309</v>
+      </c>
+      <c r="I32">
+        <v>0.99821428571428505</v>
+      </c>
+      <c r="J32" t="s">
+        <v>310</v>
+      </c>
+      <c r="K32">
+        <v>0.77124999999999999</v>
+      </c>
+      <c r="L32" t="s">
+        <v>311</v>
+      </c>
+      <c r="M32">
+        <v>0.74124999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <f>AVERAGE(K28:K32)</f>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="L33" t="e">
+        <f t="shared" ref="L33:M33" si="0">AVERAGE(L28:L32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>0.74049999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <f>STDEV(K28:K32)</f>
+        <v>6.4590053413819126E-3</v>
+      </c>
+      <c r="L34" t="e">
+        <f t="shared" ref="L34:M34" si="1">STDEV(L28:L32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>8.0816149376222949E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>273</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" t="s">
+        <v>312</v>
+      </c>
+      <c r="I36">
+        <v>0.99821428571428505</v>
+      </c>
+      <c r="J36" t="s">
+        <v>313</v>
+      </c>
+      <c r="K36">
+        <v>0.72375</v>
+      </c>
+      <c r="L36" t="s">
+        <v>314</v>
+      </c>
+      <c r="M36">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" t="s">
+        <v>315</v>
+      </c>
+      <c r="I37">
+        <v>0.996428571428571</v>
+      </c>
+      <c r="J37" t="s">
+        <v>316</v>
+      </c>
+      <c r="K37">
+        <v>0.72875000000000001</v>
+      </c>
+      <c r="L37" t="s">
+        <v>317</v>
+      </c>
+      <c r="M37">
+        <v>0.73375000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" t="s">
+        <v>318</v>
+      </c>
+      <c r="I38">
+        <v>0.997857142857142</v>
+      </c>
+      <c r="J38" t="s">
+        <v>319</v>
+      </c>
+      <c r="K38">
+        <v>0.73375000000000001</v>
+      </c>
+      <c r="L38" t="s">
+        <v>320</v>
+      </c>
+      <c r="M38">
+        <v>0.70625000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39">
+        <v>14</v>
+      </c>
+      <c r="G39" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" t="s">
+        <v>321</v>
+      </c>
+      <c r="I39">
+        <v>0.997857142857142</v>
+      </c>
+      <c r="J39" t="s">
+        <v>322</v>
+      </c>
+      <c r="K39">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="L39" t="s">
+        <v>323</v>
+      </c>
+      <c r="M39">
+        <v>0.73250000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40">
+        <v>19</v>
+      </c>
+      <c r="G40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" t="s">
         <v>324</v>
       </c>
-      <c r="I31">
+      <c r="I40">
         <v>0.99678571428571405</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J40" t="s">
         <v>325</v>
       </c>
-      <c r="K31">
+      <c r="K40">
         <v>0.75</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L40" t="s">
         <v>326</v>
       </c>
-      <c r="M31">
+      <c r="M40">
         <v>0.73</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K32">
-        <f>AVERAGE(K27:K31)</f>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <f>AVERAGE(K36:K40)</f>
         <v>0.73599999999999999</v>
       </c>
-      <c r="L32" t="e">
-        <f t="shared" ref="L32:M32" si="2">AVERAGE(L27:L31)</f>
+      <c r="L41" t="e">
+        <f t="shared" ref="L41:M41" si="2">AVERAGE(L36:L40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M32">
+      <c r="M41">
         <f t="shared" si="2"/>
         <v>0.72350000000000003</v>
       </c>
     </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
-      <c r="K33">
-        <f>STDEV(K27:K31)</f>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <f>STDEV(K36:K40)</f>
         <v>1.0767427733679015E-2</v>
       </c>
-      <c r="L33" t="e">
-        <f t="shared" ref="L33:M33" si="3">STDEV(L27:L31)</f>
+      <c r="L42" t="e">
+        <f t="shared" ref="L42:M42" si="3">STDEV(L36:L40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M33">
+      <c r="M42">
         <f t="shared" si="3"/>
         <v>1.2228297101395596E-2</v>
       </c>
@@ -20676,86 +20862,139 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="1" width="62.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+      <c r="B2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>367</v>
       </c>
       <c r="C3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D3" t="s">
-        <v>330</v>
-      </c>
-      <c r="E3" t="s">
-        <v>329</v>
-      </c>
-      <c r="F3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H3" t="s">
-        <v>328</v>
-      </c>
-      <c r="I3" t="s">
-        <v>333</v>
-      </c>
-      <c r="J3" t="s">
-        <v>334</v>
-      </c>
-      <c r="K3" t="s">
-        <v>333</v>
-      </c>
-      <c r="L3" t="s">
-        <v>335</v>
-      </c>
-      <c r="M3" t="s">
-        <v>336</v>
-      </c>
-      <c r="N3" t="s">
-        <v>328</v>
-      </c>
-      <c r="O3" t="s">
-        <v>337</v>
-      </c>
-      <c r="P3" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>337</v>
-      </c>
-      <c r="R3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>341</v>
+        <v>372</v>
+      </c>
+      <c r="B5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>378</v>
+      </c>
+      <c r="B9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>384</v>
+      </c>
+      <c r="B11" t="s">
+        <v>385</v>
+      </c>
+      <c r="C11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" t="s">
+        <v>388</v>
+      </c>
+      <c r="C12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>390</v>
+      </c>
+      <c r="B13" t="s">
+        <v>391</v>
+      </c>
+      <c r="C13" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
contingency matrix for CNN model
</commit_message>
<xml_diff>
--- a/data/buzzfeed-debunk-combined/visualization.xlsx
+++ b/data/buzzfeed-debunk-combined/visualization.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="rashkin classifier" sheetId="1" r:id="rId1"/>
     <sheet name="liar classifier" sheetId="2" r:id="rId2"/>
-    <sheet name="summary" sheetId="3" r:id="rId3"/>
+    <sheet name="data statistics summary" sheetId="3" r:id="rId3"/>
     <sheet name="CNN 1 500" sheetId="5" r:id="rId4"/>
     <sheet name="CNN 2 500" sheetId="4" r:id="rId5"/>
     <sheet name="CNN1 1000" sheetId="6" r:id="rId6"/>
     <sheet name="CNN2 1000" sheetId="7" r:id="rId7"/>
     <sheet name="CNN binary" sheetId="8" r:id="rId8"/>
     <sheet name="TF-IDF" sheetId="11" r:id="rId9"/>
-    <sheet name="Results Table" sheetId="10" r:id="rId10"/>
+    <sheet name="Misinf detection results table" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="380">
   <si>
     <t xml:space="preserve">ftrue </t>
   </si>
@@ -4229,10 +4229,13 @@
     <t>5-way with TFIDF NB</t>
   </si>
   <si>
-    <t>total number of items from each class in test data</t>
-  </si>
-  <si>
     <t>Total of predicted labels (indicative of bias)</t>
+  </si>
+  <si>
+    <t>Accuracy per class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test items per class </t>
   </si>
 </sst>
 </file>
@@ -4360,7 +4363,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4400,6 +4403,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4518,7 +4533,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4576,6 +4591,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5107,6 +5124,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5588,6 +5606,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6631,6 +6650,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7133,6 +7153,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15114,16 +15135,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22720,19 +22741,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="7" max="7" width="46.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>376</v>
       </c>
@@ -22752,10 +22774,13 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -22778,8 +22803,12 @@
         <f>SUM(B2:F2)</f>
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="23">
+        <f>B2/G2</f>
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -22802,8 +22831,12 @@
         <f t="shared" ref="G3:G7" si="0">SUM(B3:F3)</f>
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="23">
+        <f>C3/G3</f>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -22826,8 +22859,12 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="23">
+        <f>D4/G4</f>
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -22850,8 +22887,12 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="23">
+        <f>E5/G5</f>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -22874,10 +22915,14 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="23">
+        <f>F6/G6</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B7" s="22">
         <f>SUM(B2:B6)</f>
@@ -22902,6 +22947,10 @@
       <c r="G7">
         <f t="shared" si="0"/>
         <v>1000</v>
+      </c>
+      <c r="H7" s="24">
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.56700000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lwic / table data writing added
</commit_message>
<xml_diff>
--- a/data/buzzfeed-debunk-combined/visualization.xlsx
+++ b/data/buzzfeed-debunk-combined/visualization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="rashkin classifier" sheetId="1" r:id="rId1"/>
@@ -4428,8 +4428,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4594,7 +4598,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4646,6 +4650,8 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4697,6 +4703,8 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -16674,7 +16682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -22743,8 +22751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>